<commit_message>
modified:   excel_operate/sheet_comparison.py 	new file:   "tests/\346\257\224\350\276\203\347\244\272\344\276\213 - \345\216\237.xlsx" 	new file:   "tests/\346\257\224\350\276\203\347\244\272\344\276\213 - \345\257\271\346\257\224.xlsx" 	deleted:    "tests/\347\244\272\344\276\213 - \345\257\271\346\257\224.xlsx" 	modified:   "tests/\347\244\272\344\276\213.xlsx"
</commit_message>
<xml_diff>
--- a/tests/示例.xlsx
+++ b/tests/示例.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
   <si>
     <t>加value</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>这里的单元格是合并的</t>
+  </si>
+  <si>
+    <t>插入A</t>
+  </si>
+  <si>
+    <t>插入B</t>
   </si>
   <si>
     <t>戎保</t>
@@ -92,8 +98,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -108,6 +114,97 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -128,20 +225,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,30 +235,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,60 +255,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -283,187 +289,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,35 +542,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -580,21 +557,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -606,6 +568,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -633,6 +604,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -641,145 +647,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="13">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="11">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="10">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1273,10 +1279,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I$1:S$1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1355,128 +1361,124 @@
       </c>
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:8">
-      <c r="A4" s="13">
-        <v>2</v>
-      </c>
+      <c r="A4" s="13"/>
       <c r="B4" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="13">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="D4" s="13">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E4" s="13">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="F4" s="13">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="G4" s="13">
-        <v>95</v>
-      </c>
-      <c r="H4" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:8">
-      <c r="A5" s="13">
-        <v>3</v>
-      </c>
+      <c r="A5" s="13"/>
       <c r="B5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="13">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="D5" s="13">
+        <v>77</v>
+      </c>
+      <c r="E5" s="13">
         <v>88</v>
       </c>
-      <c r="E5" s="13">
-        <v>78</v>
-      </c>
       <c r="F5" s="13">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="G5" s="13">
-        <v>62</v>
-      </c>
-      <c r="H5" s="16"/>
+        <v>100</v>
+      </c>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:8">
       <c r="A6" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="13">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="D6" s="13">
+        <v>65</v>
+      </c>
+      <c r="E6" s="13">
+        <v>75</v>
+      </c>
+      <c r="F6" s="13">
         <v>82</v>
       </c>
-      <c r="E6" s="13">
-        <v>83</v>
-      </c>
-      <c r="F6" s="13">
-        <v>81</v>
-      </c>
       <c r="G6" s="13">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="H6" s="16"/>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:8">
       <c r="A7" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="13">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="D7" s="13">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E7" s="13">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F7" s="13">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G7" s="13">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="H7" s="16"/>
     </row>
     <row r="8" ht="25" customHeight="1" spans="1:8">
       <c r="A8" s="13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="13">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="D8" s="13">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E8" s="13">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="F8" s="13">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="13">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="H8" s="16"/>
     </row>
     <row r="9" ht="25" customHeight="1" spans="1:8">
       <c r="A9" s="13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>18</v>
@@ -1485,108 +1487,156 @@
         <v>72</v>
       </c>
       <c r="D9" s="13">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E9" s="13">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F9" s="13">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="G9" s="13">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="H9" s="16"/>
     </row>
     <row r="10" ht="25" customHeight="1" spans="1:8">
       <c r="A10" s="13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="13">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D10" s="13">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E10" s="13">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="F10" s="13">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="G10" s="13">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="H10" s="16"/>
     </row>
     <row r="11" ht="25" customHeight="1" spans="1:8">
       <c r="A11" s="13">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="13">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="D11" s="13">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="E11" s="13">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="F11" s="13">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G11" s="13">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="H11" s="16"/>
     </row>
     <row r="12" ht="25" customHeight="1" spans="1:8">
       <c r="A12" s="13">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="13">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D12" s="13">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E12" s="13">
         <v>85</v>
       </c>
       <c r="F12" s="13">
+        <v>96</v>
+      </c>
+      <c r="G12" s="13">
+        <v>98</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" ht="25" customHeight="1" spans="1:8">
+      <c r="A13" s="13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13">
+        <v>53</v>
+      </c>
+      <c r="D13" s="13">
+        <v>64</v>
+      </c>
+      <c r="E13" s="13">
+        <v>62</v>
+      </c>
+      <c r="F13" s="13">
+        <v>85</v>
+      </c>
+      <c r="G13" s="13">
+        <v>72</v>
+      </c>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" ht="25" customHeight="1" spans="1:8">
+      <c r="A14" s="13">
+        <v>10</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="13">
+        <v>65</v>
+      </c>
+      <c r="D14" s="13">
+        <v>84</v>
+      </c>
+      <c r="E14" s="13">
+        <v>85</v>
+      </c>
+      <c r="F14" s="13">
         <v>88</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G14" s="13">
         <v>95</v>
       </c>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" ht="25" customHeight="1" spans="1:8">
-      <c r="A13" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" ht="25" customHeight="1" spans="1:8">
+      <c r="A15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="H3:H12"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="H3:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1681,7 +1731,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5">
         <v>58</v>
@@ -1705,7 +1755,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5">
         <v>90</v>
@@ -1729,7 +1779,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="5">
         <v>85</v>
@@ -1753,7 +1803,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5">
         <v>72</v>
@@ -1777,7 +1827,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5">
         <v>48</v>
@@ -1801,7 +1851,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5">
         <v>72</v>
@@ -1825,7 +1875,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5">
         <v>63</v>
@@ -1849,7 +1899,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5">
         <v>53</v>
@@ -1873,7 +1923,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5">
         <v>65</v>
@@ -1894,7 +1944,7 @@
     </row>
     <row r="13" ht="25" customHeight="1" spans="1:8">
       <c r="A13" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>

</xml_diff>

<commit_message>
modified:   excel_operate/list_operate/list_operate.py 	modified:   excel_operate/sheet_comparison/sheet_comparison.py 	modified:   "tests/\347\244\272\344\276\213.xlsx"
</commit_message>
<xml_diff>
--- a/tests/示例.xlsx
+++ b/tests/示例.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
   <si>
     <t>加value</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>这里的单元格是合并的</t>
-  </si>
-  <si>
-    <t>插入A</t>
-  </si>
-  <si>
-    <t>插入B</t>
   </si>
   <si>
     <t>戎保</t>
@@ -99,8 +93,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -109,6 +103,74 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -126,26 +188,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -157,16 +212,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,66 +243,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -289,25 +283,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,157 +457,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,6 +536,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -572,11 +595,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,41 +633,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -647,10 +641,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
@@ -659,133 +653,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="13">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="11">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1279,10 +1273,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1361,124 +1355,128 @@
       </c>
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:8">
-      <c r="A4" s="13"/>
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
       <c r="B4" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="13">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="D4" s="13">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E4" s="13">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F4" s="13">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="G4" s="13">
-        <v>55</v>
-      </c>
-      <c r="H4" s="15"/>
+        <v>95</v>
+      </c>
+      <c r="H4" s="16"/>
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:8">
-      <c r="A5" s="13"/>
+      <c r="A5" s="13">
+        <v>3</v>
+      </c>
       <c r="B5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="13">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="D5" s="13">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E5" s="13">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F5" s="13">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="G5" s="13">
-        <v>100</v>
-      </c>
-      <c r="H5" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:8">
       <c r="A6" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="13">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="D6" s="13">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E6" s="13">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="F6" s="13">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6" s="13">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="H6" s="16"/>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:8">
       <c r="A7" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="13">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D7" s="13">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E7" s="13">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F7" s="13">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G7" s="13">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="H7" s="16"/>
     </row>
     <row r="8" ht="25" customHeight="1" spans="1:8">
       <c r="A8" s="13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="13">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="D8" s="13">
+        <v>75</v>
+      </c>
+      <c r="E8" s="13">
+        <v>36</v>
+      </c>
+      <c r="F8" s="13">
         <v>82</v>
       </c>
-      <c r="E8" s="13">
-        <v>83</v>
-      </c>
-      <c r="F8" s="13">
-        <v>81</v>
-      </c>
       <c r="G8" s="13">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="H8" s="16"/>
     </row>
     <row r="9" ht="25" customHeight="1" spans="1:8">
       <c r="A9" s="13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>18</v>
@@ -1487,156 +1485,108 @@
         <v>72</v>
       </c>
       <c r="D9" s="13">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E9" s="13">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F9" s="13">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="G9" s="13">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="H9" s="16"/>
     </row>
     <row r="10" ht="25" customHeight="1" spans="1:8">
       <c r="A10" s="13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="13">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D10" s="13">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" s="13">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="F10" s="13">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G10" s="13">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="H10" s="16"/>
     </row>
     <row r="11" ht="25" customHeight="1" spans="1:8">
       <c r="A11" s="13">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="13">
+        <v>53</v>
+      </c>
+      <c r="D11" s="13">
+        <v>64</v>
+      </c>
+      <c r="E11" s="13">
+        <v>62</v>
+      </c>
+      <c r="F11" s="13">
+        <v>85</v>
+      </c>
+      <c r="G11" s="13">
         <v>72</v>
-      </c>
-      <c r="D11" s="13">
-        <v>78</v>
-      </c>
-      <c r="E11" s="13">
-        <v>82</v>
-      </c>
-      <c r="F11" s="13">
-        <v>88</v>
-      </c>
-      <c r="G11" s="13">
-        <v>89</v>
       </c>
       <c r="H11" s="16"/>
     </row>
     <row r="12" ht="25" customHeight="1" spans="1:8">
       <c r="A12" s="13">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="13">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D12" s="13">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E12" s="13">
         <v>85</v>
       </c>
       <c r="F12" s="13">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G12" s="13">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H12" s="16"/>
     </row>
     <row r="13" ht="25" customHeight="1" spans="1:8">
-      <c r="A13" s="13">
-        <v>9</v>
-      </c>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="13">
-        <v>53</v>
-      </c>
-      <c r="D13" s="13">
-        <v>64</v>
-      </c>
-      <c r="E13" s="13">
-        <v>62</v>
-      </c>
-      <c r="F13" s="13">
-        <v>85</v>
-      </c>
-      <c r="G13" s="13">
-        <v>72</v>
-      </c>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" ht="25" customHeight="1" spans="1:8">
-      <c r="A14" s="13">
-        <v>10</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="13">
-        <v>65</v>
-      </c>
-      <c r="D14" s="13">
-        <v>84</v>
-      </c>
-      <c r="E14" s="13">
-        <v>85</v>
-      </c>
-      <c r="F14" s="13">
-        <v>88</v>
-      </c>
-      <c r="G14" s="13">
-        <v>95</v>
-      </c>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" ht="25" customHeight="1" spans="1:8">
-      <c r="A15" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="H3:H14"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="H3:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1731,7 +1681,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5">
         <v>58</v>
@@ -1755,7 +1705,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5">
         <v>90</v>
@@ -1779,7 +1729,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5">
         <v>85</v>
@@ -1803,7 +1753,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="5">
         <v>72</v>
@@ -1827,7 +1777,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="5">
         <v>48</v>
@@ -1851,7 +1801,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5">
         <v>72</v>
@@ -1875,7 +1825,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5">
         <v>63</v>
@@ -1899,7 +1849,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5">
         <v>53</v>
@@ -1923,7 +1873,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="5">
         <v>65</v>
@@ -1944,7 +1894,7 @@
     </row>
     <row r="13" ht="25" customHeight="1" spans="1:8">
       <c r="A13" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>

</xml_diff>